<commit_message>
maj code suite à des problème instabilité du can lors de l'init
</commit_message>
<xml_diff>
--- a/Fiche-Carte.xlsx
+++ b/Fiche-Carte.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F85D74-69AF-49EC-8F98-9360554B4FAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79439AB1-DBB0-486B-98DE-8ADBE3E7D080}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="742" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="742" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Généralités" sheetId="8" r:id="rId1"/>
     <sheet name="Fonctionnement" sheetId="1" r:id="rId2"/>
     <sheet name="Entrées-Sorties" sheetId="4" r:id="rId3"/>
-    <sheet name="Comoposants" sheetId="11" r:id="rId4"/>
+    <sheet name="Composants" sheetId="11" r:id="rId4"/>
     <sheet name="Docs utile" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="144">
   <si>
     <r>
       <t>Identification de la carte :</t>
@@ -398,15 +398,9 @@
     <t>Palette gauche</t>
   </si>
   <si>
-    <t>Palette ChipSelect</t>
-  </si>
-  <si>
     <t>IntpinCAN</t>
   </si>
   <si>
-    <t>A3</t>
-  </si>
-  <si>
     <t>analogique</t>
   </si>
   <si>
@@ -540,6 +534,9 @@
   </si>
   <si>
     <t xml:space="preserve">Motoréducteur </t>
+  </si>
+  <si>
+    <t>ChipSelect</t>
   </si>
 </sst>
 </file>
@@ -930,6 +927,69 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -967,134 +1027,71 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2029,7 +2026,7 @@
   </sheetPr>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
@@ -2042,69 +2039,69 @@
       <c r="A1" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="21">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="26" t="s">
+      <c r="B3" s="48"/>
+      <c r="C3" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="29" t="s">
+      <c r="B5" s="48"/>
+      <c r="C5" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28" t="s">
+      <c r="B9" s="50"/>
+      <c r="C9" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="29" t="s">
+      <c r="B11" s="50"/>
+      <c r="C11" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="29" t="s">
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="14"/>
@@ -2123,163 +2120,163 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="29" t="s">
+      <c r="B16" s="50"/>
+      <c r="C16" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="31" t="s">
+      <c r="B20" s="55"/>
+      <c r="C20" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="32"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="29">
+      <c r="B23" s="53"/>
+      <c r="C23" s="52">
         <v>18</v>
       </c>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="29" t="s">
+      <c r="B25" s="48"/>
+      <c r="C25" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="28" t="s">
+      <c r="B27" s="48"/>
+      <c r="C27" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="13"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="25"/>
+      <c r="B33" s="48"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="F34" s="31" t="s">
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
+      <c r="F34" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="54"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="F35" s="31" t="s">
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="F35" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="54"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="F36" s="31" t="s">
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="F36" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="54"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="F37" s="31" t="s">
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="F37" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="32">
@@ -2334,7 +2331,7 @@
   </sheetPr>
   <dimension ref="A2:P46"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A8" zoomScale="80" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A22" zoomScale="80" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -2355,8 +2352,8 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="15.6" customHeight="1">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
       <c r="E2" s="18"/>
@@ -2364,89 +2361,89 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:16" ht="15.75">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="58"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="19"/>
       <c r="F3" s="17"/>
       <c r="H3" s="6"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15.6" customHeight="1">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="17"/>
       <c r="E4" s="18"/>
       <c r="F4" s="17"/>
       <c r="H4" s="6"/>
       <c r="K4" s="6"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
     </row>
     <row r="5" spans="1:16" ht="15.6" customHeight="1">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
       <c r="E5" s="18"/>
       <c r="F5" s="17"/>
       <c r="H5" s="6"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
       <c r="H6" s="6"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="A7" s="59"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
       <c r="H7" s="6"/>
       <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="A8" s="59"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
       <c r="H8" s="6"/>
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:16" ht="81.75" customHeight="1">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:16">
@@ -2460,11 +2457,11 @@
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:16" ht="15.75">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
       <c r="E12" s="6"/>
       <c r="G12" s="3"/>
       <c r="H12" s="6"/>
@@ -2475,59 +2472,59 @@
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:16" ht="15" customHeight="1">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:16" ht="15" customHeight="1">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
     </row>
     <row r="18" spans="1:8" ht="44.25" customHeight="1">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
+      <c r="A18" s="57"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
     </row>
     <row r="19" spans="1:8">
       <c r="B19" s="6"/>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:8" ht="15.75">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:8">
@@ -2535,62 +2532,62 @@
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
     </row>
     <row r="23" spans="1:8" ht="14.25">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1">
-      <c r="A25" s="34"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1">
-      <c r="A26" s="34"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="A26" s="57"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1">
-      <c r="A27" s="34"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:8">
@@ -2598,30 +2595,30 @@
       <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
     </row>
     <row r="31" spans="1:8" ht="14.25">
-      <c r="A31" s="34"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1">
-      <c r="A32" s="34"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:6">
@@ -2641,46 +2638,46 @@
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1">
-      <c r="A37" s="34"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="A37" s="57"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
     </row>
     <row r="38" spans="1:6" ht="14.25">
-      <c r="A38" s="34"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
+      <c r="A38" s="57"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
     </row>
     <row r="39" spans="1:6" ht="14.25">
-      <c r="A39" s="34"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
+      <c r="A39" s="57"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="57"/>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1">
-      <c r="A40" s="34"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
+      <c r="A40" s="57"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="57"/>
     </row>
     <row r="41" spans="1:6">
       <c r="B41" s="6"/>
@@ -2738,8 +2735,8 @@
   </sheetPr>
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="115" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:B38"/>
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="90" zoomScaleNormal="115" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -2755,19 +2752,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.399999999999999" customHeight="1">
-      <c r="A1" s="42"/>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
       <c r="D2" s="10"/>
       <c r="E2" s="9"/>
       <c r="N2" s="10"/>
@@ -2778,23 +2775,23 @@
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:14" ht="30" customHeight="1" thickBot="1">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="73" t="s">
+      <c r="B4" s="67"/>
+      <c r="C4" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="75" t="s">
+      <c r="E4" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="75" t="s">
+      <c r="F4" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="76" t="s">
+      <c r="G4" s="47" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2803,619 +2800,619 @@
         <v>44</v>
       </c>
       <c r="B5" s="69"/>
-      <c r="C5" s="70" t="s">
+      <c r="C5" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="71" t="s">
+      <c r="D5" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="71" t="s">
+      <c r="E5" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71">
+      <c r="F5" s="44"/>
+      <c r="G5" s="44">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="50" t="s">
+      <c r="B6" s="71"/>
+      <c r="C6" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49">
+      <c r="F6" s="29"/>
+      <c r="G6" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="39"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="49" t="s">
+      <c r="E7" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="49" t="s">
+      <c r="F7" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="49">
+      <c r="G7" s="29">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="39"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="49">
+      <c r="G8" s="29">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="46" t="s">
+      <c r="B9" s="63"/>
+      <c r="C9" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="49">
+      <c r="G9" s="29">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.399999999999999" customHeight="1">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="39"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49">
+      <c r="F10" s="29"/>
+      <c r="G10" s="29">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.399999999999999" customHeight="1">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="39"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="E11" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49">
+      <c r="F11" s="29"/>
+      <c r="G11" s="29">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="29.25" customHeight="1">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="46" t="s">
+      <c r="B12" s="63"/>
+      <c r="C12" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="49" t="s">
+      <c r="F12" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="49"/>
+      <c r="G12" s="29"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="46" t="s">
+      <c r="B13" s="63"/>
+      <c r="C13" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="49" t="s">
+      <c r="E13" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="49" t="s">
+      <c r="F13" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="49"/>
+      <c r="G13" s="29"/>
     </row>
     <row r="14" spans="1:14" ht="30" customHeight="1">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="53" t="s">
+      <c r="B14" s="73"/>
+      <c r="C14" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="54" t="s">
+      <c r="E14" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="54" t="s">
+      <c r="F14" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="G14" s="54" t="s">
+      <c r="G14" s="32" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="18.399999999999999" customHeight="1">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="46" t="s">
+      <c r="B15" s="63"/>
+      <c r="C15" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="49" t="s">
+      <c r="E15" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="49" t="s">
+      <c r="F15" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="49" t="s">
+      <c r="G15" s="29" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="39"/>
+      <c r="B16" s="63"/>
       <c r="C16" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D16" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="49" t="s">
+      <c r="E16" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F16" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="G16" s="49" t="s">
+      <c r="G16" s="29" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18.399999999999999" customHeight="1">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="39"/>
+      <c r="B17" s="63"/>
       <c r="C17" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="49" t="s">
+      <c r="D17" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="49" t="s">
+      <c r="E17" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="49" t="s">
+      <c r="F17" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="49" t="s">
+      <c r="G17" s="29" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18.399999999999999" customHeight="1">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="39"/>
+      <c r="B18" s="63"/>
       <c r="C18" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="49" t="s">
+      <c r="E18" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="49" t="s">
+      <c r="F18" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="G18" s="49" t="s">
+      <c r="G18" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="H18" s="47"/>
+      <c r="H18" s="27"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="39"/>
+      <c r="B19" s="63"/>
       <c r="C19" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="49" t="s">
+      <c r="D19" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="49" t="s">
+      <c r="E19" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F19" s="49" t="s">
+      <c r="F19" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="49" t="s">
+      <c r="G19" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="H19" s="47"/>
+      <c r="H19" s="27"/>
     </row>
     <row r="20" spans="1:8" ht="18.399999999999999" customHeight="1">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="39"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="49" t="s">
+      <c r="E20" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="49" t="s">
+      <c r="F20" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="G20" s="49" t="s">
+      <c r="G20" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H20" s="47"/>
+      <c r="H20" s="27"/>
     </row>
     <row r="21" spans="1:8" ht="18.399999999999999" customHeight="1">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="39"/>
+      <c r="B21" s="63"/>
       <c r="C21" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="49" t="s">
+      <c r="D21" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="49" t="s">
+      <c r="E21" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="49" t="s">
+      <c r="F21" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G21" s="49" t="s">
+      <c r="G21" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H21" s="47"/>
+      <c r="H21" s="27"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="39"/>
+      <c r="B22" s="63"/>
       <c r="C22" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D22" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="49" t="s">
+      <c r="E22" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="49" t="s">
+      <c r="F22" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="G22" s="49" t="s">
+      <c r="G22" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="H22" s="48"/>
+      <c r="H22" s="28"/>
     </row>
     <row r="23" spans="1:8">
       <c r="B23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="H23" s="48"/>
+      <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:8">
       <c r="E24" s="9"/>
-      <c r="H24" s="48"/>
+      <c r="H24" s="28"/>
     </row>
     <row r="25" spans="1:8" ht="18.399999999999999" customHeight="1">
       <c r="A25" s="24"/>
       <c r="B25" s="24"/>
       <c r="C25" s="24"/>
       <c r="E25" s="9"/>
-      <c r="H25" s="48"/>
+      <c r="H25" s="28"/>
     </row>
     <row r="26" spans="1:8" ht="18.399999999999999" customHeight="1">
-      <c r="A26" s="55" t="s">
+      <c r="A26" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="58"/>
-      <c r="H26" s="48"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="33"/>
+      <c r="H26" s="28"/>
     </row>
     <row r="27" spans="1:8" ht="18.399999999999999" customHeight="1" thickBot="1">
-      <c r="H27" s="48"/>
+      <c r="H27" s="28"/>
     </row>
     <row r="28" spans="1:8" ht="18.399999999999999" customHeight="1" thickBot="1">
-      <c r="A28" s="80" t="s">
+      <c r="A28" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="81"/>
-      <c r="C28" s="78" t="s">
+      <c r="B28" s="76"/>
+      <c r="C28" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="79"/>
-      <c r="E28" s="78" t="s">
+      <c r="D28" s="78"/>
+      <c r="E28" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="F28" s="79"/>
-      <c r="H28" s="48"/>
+      <c r="F28" s="78"/>
+      <c r="H28" s="28"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1">
-      <c r="A29" s="77" t="s">
+      <c r="A29" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="77"/>
-      <c r="C29" s="77" t="s">
+      <c r="B29" s="79"/>
+      <c r="C29" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="77"/>
-      <c r="E29" s="77" t="s">
+      <c r="D29" s="79"/>
+      <c r="E29" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="F29" s="77"/>
-      <c r="H29" s="48"/>
+      <c r="F29" s="79"/>
+      <c r="H29" s="28"/>
     </row>
     <row r="30" spans="1:8" ht="18.399999999999999" customHeight="1">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56" t="s">
+      <c r="B30" s="61"/>
+      <c r="C30" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56" t="s">
+      <c r="D30" s="61"/>
+      <c r="E30" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="F30" s="56"/>
-      <c r="H30" s="48"/>
+      <c r="F30" s="61"/>
+      <c r="H30" s="28"/>
     </row>
     <row r="31" spans="1:8" ht="18.399999999999999" customHeight="1">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56" t="s">
+      <c r="B31" s="61"/>
+      <c r="C31" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56">
+      <c r="D31" s="61"/>
+      <c r="E31" s="61">
         <v>0</v>
       </c>
-      <c r="F31" s="56"/>
-      <c r="H31" s="48"/>
+      <c r="F31" s="61"/>
+      <c r="H31" s="28"/>
     </row>
     <row r="32" spans="1:8" ht="18.399999999999999" customHeight="1">
-      <c r="A32" s="56" t="s">
+      <c r="A32" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="56"/>
-      <c r="C32" s="56" t="s">
+      <c r="B32" s="61"/>
+      <c r="C32" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56">
+      <c r="D32" s="61"/>
+      <c r="E32" s="61">
         <v>1</v>
       </c>
-      <c r="F32" s="56"/>
-      <c r="H32" s="48"/>
+      <c r="F32" s="61"/>
+      <c r="H32" s="28"/>
     </row>
     <row r="33" spans="1:8" ht="18.399999999999999" customHeight="1">
-      <c r="A33" s="56" t="s">
+      <c r="A33" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="56"/>
-      <c r="C33" s="56" t="s">
+      <c r="B33" s="61"/>
+      <c r="C33" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56" t="s">
+      <c r="D33" s="61"/>
+      <c r="E33" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="F33" s="56"/>
-      <c r="H33" s="48"/>
+      <c r="F33" s="61"/>
+      <c r="H33" s="28"/>
     </row>
     <row r="34" spans="1:8" ht="18.399999999999999" customHeight="1">
-      <c r="A34" s="56" t="s">
+      <c r="A34" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="56"/>
-      <c r="C34" s="56" t="s">
+      <c r="B34" s="61"/>
+      <c r="C34" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56">
+      <c r="D34" s="61"/>
+      <c r="E34" s="61">
         <v>3</v>
       </c>
-      <c r="F34" s="56"/>
-      <c r="H34" s="48"/>
+      <c r="F34" s="61"/>
+      <c r="H34" s="28"/>
     </row>
     <row r="35" spans="1:8" ht="18.399999999999999" customHeight="1">
-      <c r="A35" s="56" t="s">
+      <c r="A35" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="56"/>
-      <c r="C35" s="56" t="s">
+      <c r="B35" s="61"/>
+      <c r="C35" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56">
+      <c r="D35" s="61"/>
+      <c r="E35" s="61">
         <v>4</v>
       </c>
-      <c r="F35" s="56"/>
-      <c r="H35" s="48"/>
+      <c r="F35" s="61"/>
+      <c r="H35" s="28"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="74" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="57"/>
-      <c r="C36" s="56" t="s">
+      <c r="B36" s="74"/>
+      <c r="C36" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56">
+      <c r="D36" s="61"/>
+      <c r="E36" s="61">
         <v>7</v>
       </c>
-      <c r="F36" s="56"/>
-      <c r="H36" s="48"/>
+      <c r="F36" s="61"/>
+      <c r="H36" s="28"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="57" t="s">
+      <c r="A37" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="B37" s="57"/>
-      <c r="C37" s="56" t="s">
-        <v>100</v>
-      </c>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56" t="s">
-        <v>99</v>
-      </c>
-      <c r="F37" s="56"/>
-      <c r="H37" s="48"/>
+      <c r="B37" s="74"/>
+      <c r="C37" s="61" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="61"/>
+      <c r="E37" s="61">
+        <v>6</v>
+      </c>
+      <c r="F37" s="61"/>
+      <c r="H37" s="28"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="57" t="s">
+      <c r="A38" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="B38" s="57"/>
-      <c r="C38" s="56" t="s">
+      <c r="B38" s="74"/>
+      <c r="C38" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56">
+      <c r="D38" s="61"/>
+      <c r="E38" s="61">
         <v>8</v>
       </c>
-      <c r="F38" s="56"/>
-      <c r="H38" s="48"/>
+      <c r="F38" s="61"/>
+      <c r="H38" s="28"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="56" t="s">
+      <c r="A39" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="B39" s="56"/>
-      <c r="C39" s="56" t="s">
+      <c r="B39" s="61"/>
+      <c r="C39" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56">
+      <c r="D39" s="61"/>
+      <c r="E39" s="61">
         <v>9</v>
       </c>
-      <c r="F39" s="56"/>
-      <c r="H39" s="48"/>
+      <c r="F39" s="61"/>
+      <c r="H39" s="28"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="56" t="s">
+      <c r="A40" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="B40" s="61"/>
+      <c r="C40" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="61"/>
+      <c r="E40" s="61">
+        <v>10</v>
+      </c>
+      <c r="F40" s="61"/>
+      <c r="H40" s="28"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="56" t="s">
+      <c r="B41" s="61"/>
+      <c r="C41" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56">
-        <v>10</v>
-      </c>
-      <c r="F40" s="56"/>
-      <c r="H40" s="48"/>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="56" t="s">
-        <v>98</v>
-      </c>
-      <c r="B41" s="56"/>
-      <c r="C41" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56">
+      <c r="D41" s="61"/>
+      <c r="E41" s="61">
         <v>2</v>
       </c>
-      <c r="F41" s="56"/>
-      <c r="H41" s="48"/>
+      <c r="F41" s="61"/>
+      <c r="H41" s="28"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="24"/>
       <c r="B42" s="24"/>
       <c r="C42" s="24"/>
-      <c r="H42" s="48"/>
+      <c r="H42" s="28"/>
     </row>
     <row r="43" spans="1:8">
       <c r="B43" s="9"/>
-      <c r="H43" s="48"/>
+      <c r="H43" s="28"/>
     </row>
     <row r="44" spans="1:8">
       <c r="B44" s="9"/>
@@ -3471,6 +3468,11 @@
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="E28:F28"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A31:B31"/>
@@ -3479,11 +3481,6 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -3498,6 +3495,7 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A39:B39"/>
@@ -3514,7 +3512,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3534,8 +3531,8 @@
   </sheetPr>
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A3" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3572,267 +3569,267 @@
       <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:8" ht="32.25" thickBot="1">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="D6" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="E6" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="F6" s="42" t="s">
         <v>104</v>
-      </c>
-      <c r="E6" s="66" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" s="67" t="s">
-        <v>106</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="62">
+      <c r="A7" s="37">
         <v>2</v>
       </c>
-      <c r="B7" s="62" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" s="62" t="s">
-        <v>115</v>
-      </c>
-      <c r="D7" s="62" t="s">
-        <v>133</v>
-      </c>
-      <c r="E7" s="63" t="s">
-        <v>107</v>
-      </c>
-      <c r="F7" s="64"/>
+      <c r="B7" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="39"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="59">
+      <c r="A8" s="34">
         <v>1</v>
       </c>
-      <c r="B8" s="59">
+      <c r="B8" s="34">
         <v>0.5</v>
       </c>
-      <c r="C8" s="59" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="59" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" s="54" t="s">
+      <c r="C8" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="F8" s="60" t="s">
-        <v>142</v>
+      <c r="E8" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>140</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="59">
+      <c r="A9" s="34">
         <v>14</v>
       </c>
-      <c r="B9" s="59" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>117</v>
-      </c>
-      <c r="D9" s="59" t="s">
-        <v>109</v>
-      </c>
-      <c r="E9" s="54" t="s">
+      <c r="B9" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="F9" s="60"/>
+      <c r="E9" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="35"/>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="59">
+      <c r="A10" s="34">
         <v>2</v>
       </c>
-      <c r="B10" s="59" t="s">
-        <v>118</v>
-      </c>
-      <c r="C10" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="59" t="s">
-        <v>109</v>
-      </c>
-      <c r="E10" s="54" t="s">
+      <c r="B10" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="F10" s="60"/>
+      <c r="E10" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" s="35"/>
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="59">
+      <c r="A11" s="34">
         <v>1</v>
       </c>
-      <c r="B11" s="59" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" s="59" t="s">
-        <v>121</v>
-      </c>
-      <c r="D11" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="E11" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="F11" s="60"/>
+      <c r="B11" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="35"/>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="59">
+      <c r="A12" s="34">
         <v>1</v>
       </c>
-      <c r="B12" s="59" t="s">
-        <v>122</v>
-      </c>
-      <c r="C12" s="59" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="59" t="s">
-        <v>133</v>
-      </c>
-      <c r="E12" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="F12" s="60"/>
+      <c r="B12" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" s="35"/>
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="59">
+      <c r="A13" s="34">
         <v>3</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" s="59" t="s">
-        <v>135</v>
-      </c>
-      <c r="E13" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="F13" s="60" t="s">
-        <v>111</v>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>109</v>
       </c>
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="59">
+      <c r="A14" s="34">
         <v>1</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59" t="s">
-        <v>125</v>
-      </c>
-      <c r="D14" s="59" t="s">
-        <v>136</v>
-      </c>
-      <c r="E14" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="F14" s="60"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="35"/>
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="59">
+      <c r="A15" s="34">
         <v>1</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59" t="s">
-        <v>126</v>
-      </c>
-      <c r="D15" s="59" t="s">
-        <v>137</v>
-      </c>
-      <c r="E15" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="F15" s="61" t="s">
-        <v>112</v>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>110</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="59">
+      <c r="A16" s="34">
         <v>1</v>
       </c>
-      <c r="B16" s="59" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="D16" s="59" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="F16" s="60"/>
+      <c r="B16" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="35"/>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="59">
+      <c r="A17" s="34">
         <v>5</v>
       </c>
-      <c r="B17" s="59" t="s">
-        <v>129</v>
-      </c>
-      <c r="C17" s="59" t="s">
-        <v>130</v>
-      </c>
-      <c r="D17" s="59" t="s">
-        <v>138</v>
-      </c>
-      <c r="E17" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="F17" s="60" t="s">
-        <v>108</v>
+      <c r="B17" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>106</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="59">
+      <c r="A18" s="34">
         <v>1</v>
       </c>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F18" s="35" t="s">
         <v>139</v>
-      </c>
-      <c r="C18" s="59" t="s">
-        <v>131</v>
-      </c>
-      <c r="D18" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="E18" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="60" t="s">
-        <v>141</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
@@ -4171,7 +4168,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;LFiche électronique&amp;C&amp;"Century Gothic,Gras"&amp;14&amp;KFF0000Composants
 </oddHeader>
@@ -4187,8 +4184,8 @@
   </sheetPr>
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A8" zoomScale="110" zoomScaleNormal="115" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G5"/>
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="110" zoomScaleNormal="115" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4200,429 +4197,427 @@
       <c r="A1" s="15"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="82" t="s">
-        <v>144</v>
-      </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
+      <c r="A3" s="81" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="43"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="A4" s="80"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
     </row>
     <row r="5" spans="1:7" ht="13.7" customHeight="1">
-      <c r="A5" s="82" t="s">
-        <v>114</v>
-      </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
+      <c r="A5" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="44"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="82" t="s">
-        <v>143</v>
-      </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
+      <c r="A7" s="81" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
     </row>
     <row r="8" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
     </row>
     <row r="9" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
+      <c r="A9" s="80"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
     </row>
     <row r="10" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A10" s="43"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
     </row>
     <row r="11" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A11" s="43"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
+      <c r="A11" s="80"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
     </row>
     <row r="12" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A12" s="43"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="43"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
+      <c r="A13" s="80"/>
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="43"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="43"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
+      <c r="A15" s="80"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="43"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
+      <c r="A16" s="80"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="43"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
+      <c r="A17" s="80"/>
+      <c r="B17" s="80"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="80"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="43"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
+      <c r="A18" s="80"/>
+      <c r="B18" s="80"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="80"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
+      <c r="A19" s="80"/>
+      <c r="B19" s="80"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
+      <c r="A20" s="80"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="43"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
+      <c r="A21" s="80"/>
+      <c r="B21" s="80"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="80"/>
+      <c r="G21" s="80"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="43"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
+      <c r="A22" s="80"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="43"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
+      <c r="A23" s="80"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="43"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
+      <c r="A24" s="80"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="43"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
+      <c r="A25" s="80"/>
+      <c r="B25" s="80"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="80"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="43"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
+      <c r="A26" s="80"/>
+      <c r="B26" s="80"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="80"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="43"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
+      <c r="A27" s="80"/>
+      <c r="B27" s="80"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="80"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="43"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
+      <c r="A28" s="80"/>
+      <c r="B28" s="80"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="80"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="80"/>
+      <c r="G28" s="80"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="43"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
+      <c r="A29" s="80"/>
+      <c r="B29" s="80"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="80"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="80"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="43"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
+      <c r="A30" s="80"/>
+      <c r="B30" s="80"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="80"/>
+      <c r="E30" s="80"/>
+      <c r="F30" s="80"/>
+      <c r="G30" s="80"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="43"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
+      <c r="A31" s="80"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="80"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="43"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
+      <c r="A32" s="80"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="43"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
+      <c r="A33" s="80"/>
+      <c r="B33" s="80"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="43"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
+      <c r="A34" s="80"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="80"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="43"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
+      <c r="A35" s="80"/>
+      <c r="B35" s="80"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="80"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="43"/>
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
+      <c r="A36" s="80"/>
+      <c r="B36" s="80"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="80"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="43"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
+      <c r="A37" s="80"/>
+      <c r="B37" s="80"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="80"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="80"/>
+      <c r="G37" s="80"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="43"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
+      <c r="A38" s="80"/>
+      <c r="B38" s="80"/>
+      <c r="C38" s="80"/>
+      <c r="D38" s="80"/>
+      <c r="E38" s="80"/>
+      <c r="F38" s="80"/>
+      <c r="G38" s="80"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="43"/>
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
+      <c r="A39" s="80"/>
+      <c r="B39" s="80"/>
+      <c r="C39" s="80"/>
+      <c r="D39" s="80"/>
+      <c r="E39" s="80"/>
+      <c r="F39" s="80"/>
+      <c r="G39" s="80"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="43"/>
-      <c r="B40" s="43"/>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
+      <c r="A40" s="80"/>
+      <c r="B40" s="80"/>
+      <c r="C40" s="80"/>
+      <c r="D40" s="80"/>
+      <c r="E40" s="80"/>
+      <c r="F40" s="80"/>
+      <c r="G40" s="80"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="43"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
+      <c r="A41" s="80"/>
+      <c r="B41" s="80"/>
+      <c r="C41" s="80"/>
+      <c r="D41" s="80"/>
+      <c r="E41" s="80"/>
+      <c r="F41" s="80"/>
+      <c r="G41" s="80"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="43"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
+      <c r="A42" s="80"/>
+      <c r="B42" s="80"/>
+      <c r="C42" s="80"/>
+      <c r="D42" s="80"/>
+      <c r="E42" s="80"/>
+      <c r="F42" s="80"/>
+      <c r="G42" s="80"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
+      <c r="A43" s="80"/>
+      <c r="B43" s="80"/>
+      <c r="C43" s="80"/>
+      <c r="D43" s="80"/>
+      <c r="E43" s="80"/>
+      <c r="F43" s="80"/>
+      <c r="G43" s="80"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
+      <c r="A44" s="80"/>
+      <c r="B44" s="80"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="80"/>
+      <c r="E44" s="80"/>
+      <c r="F44" s="80"/>
+      <c r="G44" s="80"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
+      <c r="A45" s="80"/>
+      <c r="B45" s="80"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="80"/>
+      <c r="E45" s="80"/>
+      <c r="F45" s="80"/>
+      <c r="G45" s="80"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="43"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
+      <c r="A46" s="80"/>
+      <c r="B46" s="80"/>
+      <c r="C46" s="80"/>
+      <c r="D46" s="80"/>
+      <c r="E46" s="80"/>
+      <c r="F46" s="80"/>
+      <c r="G46" s="80"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="43"/>
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
+      <c r="A47" s="80"/>
+      <c r="B47" s="80"/>
+      <c r="C47" s="80"/>
+      <c r="D47" s="80"/>
+      <c r="E47" s="80"/>
+      <c r="F47" s="80"/>
+      <c r="G47" s="80"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="43"/>
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
+      <c r="A48" s="80"/>
+      <c r="B48" s="80"/>
+      <c r="C48" s="80"/>
+      <c r="D48" s="80"/>
+      <c r="E48" s="80"/>
+      <c r="F48" s="80"/>
+      <c r="G48" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A32:G32"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A34:G34"/>
     <mergeCell ref="A22:G22"/>
@@ -4634,11 +4629,11 @@
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="A29:G29"/>
     <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A14:G14"/>
     <mergeCell ref="A15:G15"/>
     <mergeCell ref="A16:G16"/>
     <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A32:G32"/>
     <mergeCell ref="A18:G18"/>
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="A20:G20"/>
@@ -4652,6 +4647,9 @@
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A14:G14"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="C48:E48"/>
     <mergeCell ref="F48:G48"/>
@@ -4677,24 +4675,23 @@
     <mergeCell ref="C41:E41"/>
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="F43:G43"/>
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="C44:E44"/>
     <mergeCell ref="F44:G44"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="F37:G37"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="F43:G43"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="F35:G35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="F36:G36"/>
-    <mergeCell ref="A12:G12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3:G3" r:id="rId1" display="Motoréducteur " xr:uid="{A925892E-D78F-4A30-9752-06075C799715}"/>

</xml_diff>